<commit_message>
adding support for google sheets
</commit_message>
<xml_diff>
--- a/ebay-LoadSheet.xlsx
+++ b/ebay-LoadSheet.xlsx
@@ -280,34 +280,9 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="false" diagonalDown="false">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="false" diagonalDown="false">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <diagonal/>
-      </border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -381,28 +356,27 @@
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3117408906883"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.6720647773279"/>
     <col collapsed="false" hidden="false" max="12" min="8" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="21" min="20" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="29" min="22" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="15.5303643724696"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -511,7 +485,7 @@
         <v>31</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>34532</v>
+        <v>377</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>32</v>
@@ -629,7 +603,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1000">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(TRIM(S1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
adding support for ebay seller profiles
</commit_message>
<xml_diff>
--- a/ebay-LoadSheet.xlsx
+++ b/ebay-LoadSheet.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">SKU</t>
   </si>
@@ -112,46 +112,58 @@
     <t xml:space="preserve">Best Offer</t>
   </si>
   <si>
-    <t xml:space="preserve">2354657325</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.image.com/image.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manufacturer Part Number|121313</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brand|Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interchange Part Number|</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Part Number|</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Finish|</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warranty|</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country/Region of Manufacturer|</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Years|</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ext. Years|</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicle|</t>
+    <t xml:space="preserve">JW Speaker Model 8700 Evolution J LED Headlights For 2007-2016 Jeep Wrangler JK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://blog.midwestaftermarket.com/ebay/images/8700-evo-j.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://blog.midwestaftermarket.com/ebay/images/8700-evo-j-installed.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturer Part Number|0551131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brad|JW Speaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interchange Part Number|DOT Compliant Jeep Wrangler JK Headlamp Light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Part Number|JW Speaker 8700 Evolution J Series LED Headlights 07-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Finish|Die Cast Aluminum With Black Bezel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warranty|Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country/Region of Manufacturer|United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years|07 08 09 10 11 12 13 14 15 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ext. Years|2007 2008 2009 2010 2011 2012 2013 2014 2015 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle|Jeep Wrangler JK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part Brand|12V DOT LED High &amp; Low Beam Headlights with Black Bezel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lumens|High Beam = 2,610 Low Beam = 1770</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED Color Temperature|5000K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
   </si>
 </sst>
 </file>
@@ -162,7 +174,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -191,14 +203,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -242,7 +246,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -259,15 +263,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -281,70 +281,8 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="1">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
+    <dxf/>
   </dxfs>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFB7E1CD"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -355,28 +293,31 @@
   </sheetPr>
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O6" activeCellId="0" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.3198380566802"/>
     <col collapsed="false" hidden="false" max="12" min="8" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="21" min="20" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="29" min="22" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="30.8704453441296"/>
+    <col collapsed="false" hidden="false" max="29" min="24" style="0" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="15.6396761133603"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,28 +409,35 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
-        <v>1232</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>551131</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>799475636714</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>684</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>377</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
       <c r="M2" s="4" t="s">
         <v>33</v>
       </c>
@@ -520,101 +468,117 @@
       <c r="V2" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="W2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1000">
+  <conditionalFormatting sqref="D3:D1000,D1">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(D1:D978)&gt;80</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1000">
+  <conditionalFormatting sqref="B3:B1000,B1">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(B1:B978)&gt;12</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M1000">
+  <conditionalFormatting sqref="M3:M1000,M1">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(M1:M1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1000">
+  <conditionalFormatting sqref="N3:N1000,N1">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(N1:N1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1000">
+  <conditionalFormatting sqref="O3:O1000,O1">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(O1:O1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1000">
+  <conditionalFormatting sqref="P3:P1000,P1">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(P1:P1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q1000">
+  <conditionalFormatting sqref="Q3:Q1000,Q1">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(Q1:Q1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R1000">
+  <conditionalFormatting sqref="R3:R1000,R1">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(R1:R1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T1:T1000">
+  <conditionalFormatting sqref="T3:T1000,T1">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(T1:T1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U1:U1000">
+  <conditionalFormatting sqref="U3:U1000,U1">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(U1:U1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V1:V1000">
+  <conditionalFormatting sqref="V3:V1000,V1">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(V1:V1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W1:W1000">
+  <conditionalFormatting sqref="W3:W1000,W1">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(W1:W1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X1:X1000">
+  <conditionalFormatting sqref="X3:X1000,X1">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(X1:X1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y1:Y1000">
+  <conditionalFormatting sqref="Y3:Y1000,Y1">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(Y1:Y1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z1:Z1000">
+  <conditionalFormatting sqref="Z3:Z1000,Z1">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(Z1:Z1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA1:AA1000">
+  <conditionalFormatting sqref="AA3:AA1000,AA1">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(AA1:AA1000)&gt;65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S1000">
+  <conditionalFormatting sqref="S3:S1000,S1">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(TRIM(S1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" prompt="Enter a number between 1 and 100000" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C1:C2" type="decimal">
+    <dataValidation allowBlank="true" operator="between" prompt="Enter a number between 1 and 100000" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C1" type="decimal">
       <formula1>1</formula1>
       <formula2>100000</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="http://www.image.com/image.png"/>
+    <hyperlink ref="G2" r:id="rId1" display="http://blog.midwestaftermarket.com/ebay/images/8700-evo-j.png"/>
+    <hyperlink ref="H2" r:id="rId2" display="http://blog.midwestaftermarket.com/ebay/images/8700-evo-j-installed.png"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Support to add multiple item images
</commit_message>
<xml_diff>
--- a/ebay-LoadSheet.xlsx
+++ b/ebay-LoadSheet.xlsx
@@ -130,10 +130,10 @@
     <t xml:space="preserve">Brad|JW Speaker</t>
   </si>
   <si>
-    <t xml:space="preserve">Interchange Part Number|DOT Compliant Jeep Wrangler JK Headlamp Light</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Part Number|JW Speaker 8700 Evolution J Series LED Headlights 07-16</t>
+    <t xml:space="preserve">Interchange Part Number|DOT Compliant Jeep Wrangler </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Part Number|JW Speaker 8700 Evolution </t>
   </si>
   <si>
     <t xml:space="preserve">Surface Finish|Die Cast Aluminum With Black Bezel</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">Vehicle|Jeep Wrangler JK </t>
   </si>
   <si>
-    <t xml:space="preserve">Part Brand|12V DOT LED High &amp; Low Beam Headlights with Black Bezel</t>
+    <t xml:space="preserve">Part Brand|12V DOT LED High &amp; Low Beam Headlights </t>
   </si>
   <si>
     <t xml:space="preserve">Lumens|High Beam = 2,610 Low Beam = 1770</t>
@@ -293,31 +293,31 @@
   </sheetPr>
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O6" activeCellId="0" sqref="O6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W11" activeCellId="0" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.668016194332"/>
     <col collapsed="false" hidden="false" max="12" min="8" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="21" min="20" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="30.8704453441296"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="29" min="24" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="15.7449392712551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,91 +485,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:D1000,D1">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(D1:D978)&gt;80</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B1000,B1">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B1:B978)&gt;12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M1000,M1">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(M1:M1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N1000,N1">
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(N1:N1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O1000,O1">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(O1:O1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P1000,P1">
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(P1:P1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q1000,Q1">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(Q1:Q1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R1000,R1">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(R1:R1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T3:T1000,T1">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(T1:T1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U3:U1000,U1">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(U1:U1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V1000,V1">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(V1:V1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W3:W1000,W1">
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(W1:W1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X3:X1000,X1">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(X1:X1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y1000,Y1">
-    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(Y1:Y1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z3:Z1000,Z1">
-    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(Z1:Z1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA3:AA1000,AA1">
-    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(AA1:AA1000)&gt;65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S1000,S1">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(TRIM(S1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" prompt="Enter a number between 1 and 100000" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C1" type="decimal">
       <formula1>1</formula1>

</xml_diff>